<commit_message>
Work at Starbucks on MLK
</commit_message>
<xml_diff>
--- a/Masters Thesis Tasks.xlsx
+++ b/Masters Thesis Tasks.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mengstr1\Documents\GitHub\masters-thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\drumming-robot-masters-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Compare my results with Paper</t>
   </si>
@@ -60,12 +60,18 @@
   </si>
   <si>
     <t>Request timed out, need to resubmit</t>
+  </si>
+  <si>
+    <t>Project runs, Serial comm issues</t>
+  </si>
+  <si>
+    <t>Resubmitted, was upgraded to 2008b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -481,7 +487,7 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +566,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -572,7 +580,9 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
MATLAB serial fix, Orangutan and Atmel info
Fixed serial errors with MATLAB code, added code to Word document.
Added Pololu Orangutan and Atmel AVR documentation.
</commit_message>
<xml_diff>
--- a/Masters Thesis Tasks.xlsx
+++ b/Masters Thesis Tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Compare my results with Paper</t>
   </si>
@@ -66,13 +66,76 @@
   </si>
   <si>
     <t>Resubmitted, was upgraded to 2008b</t>
+  </si>
+  <si>
+    <t>Fix serial errors</t>
+  </si>
+  <si>
+    <t>SerBEAT = serial(str); %&lt;--change this appropriately</t>
+  </si>
+  <si>
+    <t>set(SerBEAT,'BaudRate', 9600, 'DataBits', 8, 'Parity', 'none','StopBits', 1, 'FlowControl', 'none');</t>
+  </si>
+  <si>
+    <t>fopen(SerBEAT); %--open the serial port to the PIC</t>
+  </si>
+  <si>
+    <t>NOTE: try using 'serial' call with static members. Ex:</t>
+  </si>
+  <si>
+    <t>s = serial('COM1','baudrate',4800);
+OR: s2 = serial('COM2','BaudRate',1200,'DataBits',7);</t>
+  </si>
+  <si>
+    <t>query for member values:</t>
+  </si>
+  <si>
+    <t>get(s1,{'Type','Name','Port'})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ans = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    'serial'    'Serial-COM1'    'COM1'</t>
+  </si>
+  <si>
+    <t>UPDATE: fixed by using</t>
+  </si>
+  <si>
+    <r>
+      <t>upper(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COM Port String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>to make string capitals. Don't ask why it needs it, just accept it.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,13 +143,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF404040"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -153,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -169,6 +258,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -484,16 +585,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J7"/>
+  <dimension ref="A2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J15:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="10" width="19.140625" style="1" customWidth="1"/>
+    <col min="2" max="9" width="19.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="123.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -525,7 +627,9 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -541,7 +645,9 @@
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
@@ -555,7 +661,9 @@
       <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="2"/>
+      <c r="J4" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -569,7 +677,9 @@
       <c r="I5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="2"/>
+      <c r="J5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -583,9 +693,11 @@
       <c r="I6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -595,7 +707,44 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>